<commit_message>
Se ha añadido método que genera los bonus
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360E695F-43BC-4FF4-9DE8-7E9C651D4687}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6552A1E-5E6F-4404-889D-DD825F04DAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Pelotas</t>
   </si>
   <si>
-    <t>Mejoras</t>
-  </si>
-  <si>
     <t>Sprite</t>
   </si>
   <si>
@@ -169,13 +166,55 @@
   </si>
   <si>
     <t>HiloMejora</t>
+  </si>
+  <si>
+    <t>HiloPelotas</t>
+  </si>
+  <si>
+    <t>UsuarioNoExiste</t>
+  </si>
+  <si>
+    <t>PuntajeNoExiste</t>
+  </si>
+  <si>
+    <t>IOException</t>
+  </si>
+  <si>
+    <t>NumerFormatException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClassNotFound </t>
+  </si>
+  <si>
+    <t>Partida guardada</t>
+  </si>
+  <si>
+    <t>Datos de la partida guardada</t>
+  </si>
+  <si>
+    <t>Por nombre</t>
+  </si>
+  <si>
+    <t>Por puntaje</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Decoraciones</t>
+  </si>
+  <si>
+    <t>Colisionable</t>
+  </si>
+  <si>
+    <t>Movible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +227,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -231,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -256,18 +301,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="5">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -288,26 +334,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -610,7 +636,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +810,7 @@
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -798,13 +824,16 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,7 +848,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -846,10 +875,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -862,8 +891,12 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
@@ -875,8 +908,12 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
@@ -902,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -919,15 +956,17 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="8"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -938,11 +977,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -952,10 +993,14 @@
       <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -965,9 +1010,15 @@
       <c r="B11" s="1">
         <v>4</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="9"/>
     </row>
@@ -978,10 +1029,12 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -991,15 +1044,17 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -1007,6 +1062,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1015,7 +1071,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1112,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Las pelotas se generan, se mueven en la pantalla y rebotan. Se detecta la colision con la nave
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6552A1E-5E6F-4404-889D-DD825F04DAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D8A4E12F-5E99-4E5D-B0F0-76D277072821}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Movible</t>
+  </si>
+  <si>
+    <t>Ver si hay colision con alguna pelota</t>
+  </si>
+  <si>
+    <t>Crear arreglo de pelotas</t>
   </si>
 </sst>
 </file>
@@ -235,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -302,11 +314,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -807,10 +862,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -823,16 +878,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="5" customWidth="1"/>
   </cols>
@@ -926,8 +981,12 @@
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="9"/>
     </row>
@@ -1054,10 +1113,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1112,7 +1187,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Se añadio metodos e hilos para el manejo de las Bonificaciones (Aun no funciona la colision), y tambien se añadio el manejo de archivos de texto
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6552A1E-5E6F-4404-889D-DD825F04DAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D3336A-1B9E-4F91-AA21-E2DDE62D0A4B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +786,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,9 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Añadido metodos para el manejo del arbol de jugadores
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D8A4E12F-5E99-4E5D-B0F0-76D277072821}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8F2D4-B72B-4BC8-8DF7-F640E9FDE343}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Arboles binarios</t>
   </si>
   <si>
-    <t>Estructuras recursivas</t>
-  </si>
-  <si>
     <t>Herencias</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t>Crear arreglo de pelotas</t>
+  </si>
+  <si>
+    <t>NivelNoExiste</t>
+  </si>
+  <si>
+    <t>FileNotFoundException</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -313,15 +316,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -339,6 +353,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -389,26 +413,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -691,7 +695,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +845,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,7 +853,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,11 +866,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -876,19 +880,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -900,10 +905,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -916,8 +921,12 @@
       <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="9"/>
@@ -927,16 +936,16 @@
         <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -944,15 +953,15 @@
         <v>25</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
     </row>
@@ -961,16 +970,16 @@
         <v>26</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,54 +987,54 @@
         <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="D7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>48</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1033,15 +1042,17 @@
         <v>30</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>
@@ -1050,35 +1061,35 @@
         <v>31</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1088,7 +1099,7 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="8"/>
@@ -1096,43 +1107,28 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1157,37 +1153,37 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update en los ToDo
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8F2D4-B72B-4BC8-8DF7-F640E9FDE343}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4EBC2-59E3-412C-BBF0-D733EA2F2B7D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Diseño de casos de pruebas</t>
   </si>
   <si>
-    <t>Digrama de objetos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Peristencia </t>
   </si>
   <si>
@@ -217,6 +214,15 @@
   </si>
   <si>
     <t>FileNotFoundException</t>
+  </si>
+  <si>
+    <t>CompareTo</t>
+  </si>
+  <si>
+    <t>Diagrama de clases</t>
+  </si>
+  <si>
+    <t>Daigrama de objetos</t>
   </si>
 </sst>
 </file>
@@ -694,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +763,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,7 +779,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -797,7 +803,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +867,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -882,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,15 +910,17 @@
       <c r="B1" s="1">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
+      <c r="G1" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -922,10 +930,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -939,12 +947,14 @@
         <v>3</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
     </row>
@@ -955,15 +965,17 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -974,10 +986,10 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="9"/>
@@ -989,8 +1001,8 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
+      <c r="C6" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -1007,16 +1019,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G7" s="9"/>
     </row>
@@ -1028,10 +1040,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1045,13 +1057,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
@@ -1064,43 +1076,45 @@
         <v>4</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="F10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>53</v>
+      <c r="C11" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1139,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAF6AF0-D333-485E-AC0B-0E3E3439BB4E}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,21 +1179,27 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Diseño de pruebas para busqueda, ordenamiento y adicion de jugadores
Ahora los jugadores se ordenan por Nombre en el arbol binario
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4EBC2-59E3-412C-BBF0-D733EA2F2B7D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F860E5C-5994-416A-BD7E-A8A3E6C988D6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -165,9 +165,6 @@
     <t>HiloPelotas</t>
   </si>
   <si>
-    <t>UsuarioNoExiste</t>
-  </si>
-  <si>
     <t>PuntajeNoExiste</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>Crear arreglo de pelotas</t>
   </si>
   <si>
-    <t>NivelNoExiste</t>
-  </si>
-  <si>
     <t>FileNotFoundException</t>
   </si>
   <si>
@@ -223,6 +217,18 @@
   </si>
   <si>
     <t>Daigrama de objetos</t>
+  </si>
+  <si>
+    <t>NombreNoExiste</t>
+  </si>
+  <si>
+    <t>buscarJugadorPuntos</t>
+  </si>
+  <si>
+    <t>JugadorRepetidoException</t>
+  </si>
+  <si>
+    <t>vale si es de la manera recursiva?</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +272,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,6 +339,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,7 +714,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,10 +899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,12 +911,12 @@
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -922,7 +935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -939,7 +952,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -947,54 +960,59 @@
         <v>3</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
+      <c r="E3" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="D5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1032,7 +1050,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1040,35 +1058,35 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>62</v>
+      <c r="E9" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1076,20 +1094,20 @@
         <v>4</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="F10" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1097,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1106,7 +1124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1114,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1179,13 +1197,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="6"/>
     </row>

</xml_diff>

<commit_message>
Done el actualizar lista
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F860E5C-5994-416A-BD7E-A8A3E6C988D6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7F53B8-BB7F-4126-9F83-6C2FBE890C84}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,7 +714,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Actualizado el to-do"
This reverts commit c825b7cd35743795125ff018770b0320811c7165.
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E8C0022-0B9B-45ED-A155-94F262E699A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E646116C-F25F-4826-B65E-19A101327464}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Actualizado el to-do""
This reverts commit 84660e1198d572e3df6c3453945fa2723285b7ba.
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E646116C-F25F-4826-B65E-19A101327464}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E8C0022-0B9B-45ED-A155-94F262E699A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Añadido panel con los datos del jugador
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E8C0022-0B9B-45ED-A155-94F262E699A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6DC2C8CE-07D3-4E81-BD4C-D7BAD1247FA9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -704,7 +704,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aumenta el puntaje tras eliminar una pelota
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6DC2C8CE-07D3-4E81-BD4C-D7BAD1247FA9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F80E114D-F23F-4E78-938C-E26D5FFDDAF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -704,7 +704,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se puede subir de nivel
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F80E114D-F23F-4E78-938C-E26D5FFDDAF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ADC6AB5D-98DF-4866-AF33-5C70A822C264}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Comparable</t>
+  </si>
+  <si>
+    <t>Ver si hay pelotas vivas</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +825,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1001,9 @@
       <c r="E5" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="G5" s="9" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Creado metodos que recuperan y exportan la partida actual
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ADC6AB5D-98DF-4866-AF33-5C70A822C264}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925AC1DF-9A35-4515-A483-DD72A04AD7DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -707,7 +707,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Documentación de la clase Juego hecha
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDC0B53-3D7D-4393-8258-758793A590D1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336B56A-FCE7-4C88-8995-5D7BD2CE28ED}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
     <sheet name="Must Have" sheetId="2" r:id="rId2"/>
     <sheet name="Entregables" sheetId="3" r:id="rId3"/>
+    <sheet name="Pruebas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="126">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -210,9 +211,6 @@
     <t>Diagrama de clases</t>
   </si>
   <si>
-    <t>Daigrama de objetos</t>
-  </si>
-  <si>
     <t>NombreNoExiste</t>
   </si>
   <si>
@@ -232,6 +230,177 @@
   </si>
   <si>
     <t xml:space="preserve">Jpanel </t>
+  </si>
+  <si>
+    <t>Bonificacion</t>
+  </si>
+  <si>
+    <t>Juego</t>
+  </si>
+  <si>
+    <t>Jugador</t>
+  </si>
+  <si>
+    <t>Nave</t>
+  </si>
+  <si>
+    <t>Pelota</t>
+  </si>
+  <si>
+    <t>darDecoraciones</t>
+  </si>
+  <si>
+    <t>agregarDecoracion</t>
+  </si>
+  <si>
+    <t>crearDecoraciones</t>
+  </si>
+  <si>
+    <t>disparar</t>
+  </si>
+  <si>
+    <t>buscarJugadorNombre</t>
+  </si>
+  <si>
+    <t>toArrayListJugador</t>
+  </si>
+  <si>
+    <t>addJugador</t>
+  </si>
+  <si>
+    <t>verificarColisionProyectil</t>
+  </si>
+  <si>
+    <t>subirNivel</t>
+  </si>
+  <si>
+    <t>aumentarPuntaje</t>
+  </si>
+  <si>
+    <t>verificarColisionNave</t>
+  </si>
+  <si>
+    <t>verificarVidas</t>
+  </si>
+  <si>
+    <t>cicloJuego</t>
+  </si>
+  <si>
+    <t>ordenarNivelDescendente</t>
+  </si>
+  <si>
+    <t>ordenarNivelAscendente</t>
+  </si>
+  <si>
+    <t>ordenarPuntosDescendente</t>
+  </si>
+  <si>
+    <t>ordenarPuntosAscendente</t>
+  </si>
+  <si>
+    <t>ordenarNombreDescendente</t>
+  </si>
+  <si>
+    <t>ordenarNombreAscendente</t>
+  </si>
+  <si>
+    <t>bonusPuntaje</t>
+  </si>
+  <si>
+    <t>verificarColisionBonus</t>
+  </si>
+  <si>
+    <t>crearBonus</t>
+  </si>
+  <si>
+    <t>cargarDatos</t>
+  </si>
+  <si>
+    <t>guardarDatos</t>
+  </si>
+  <si>
+    <t>recuperarJugadores</t>
+  </si>
+  <si>
+    <t>recuperarNave</t>
+  </si>
+  <si>
+    <t>recuperarDeco</t>
+  </si>
+  <si>
+    <t>recuperarBonus</t>
+  </si>
+  <si>
+    <t>recuperarPelotas</t>
+  </si>
+  <si>
+    <t>cargarPartida</t>
+  </si>
+  <si>
+    <t>guardarDeco</t>
+  </si>
+  <si>
+    <t>guardarBonificaciones</t>
+  </si>
+  <si>
+    <t>guadarPelotas</t>
+  </si>
+  <si>
+    <t>guardarNave</t>
+  </si>
+  <si>
+    <t>guardarJugadores</t>
+  </si>
+  <si>
+    <t>guardarPartida</t>
+  </si>
+  <si>
+    <t>iniciarPelotas</t>
+  </si>
+  <si>
+    <t>insertarPelotas</t>
+  </si>
+  <si>
+    <t>Diagrama de objetos</t>
+  </si>
+  <si>
+    <t>iniciarJuego</t>
+  </si>
+  <si>
+    <t>insertar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iniciarjuego </t>
+  </si>
+  <si>
+    <t xml:space="preserve">localizarUltimoBonus </t>
+  </si>
+  <si>
+    <t>colisionaCon</t>
+  </si>
+  <si>
+    <t>hayColision</t>
+  </si>
+  <si>
+    <t>colsionaCon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hayVivas </t>
+  </si>
+  <si>
+    <t>existenColisiones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jugador </t>
+  </si>
+  <si>
+    <t>buscarNombre</t>
+  </si>
+  <si>
+    <t>buscarPuntos</t>
+  </si>
+  <si>
+    <t>agregardecoracion</t>
   </si>
 </sst>
 </file>
@@ -280,7 +449,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -342,12 +511,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -888,10 +1070,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -905,7 +1087,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,11 +1133,11 @@
       <c r="D2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>20</v>
@@ -975,7 +1157,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
@@ -1009,7 +1191,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>58</v>
@@ -1018,7 +1200,7 @@
         <v>59</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>20</v>
@@ -1074,12 +1256,14 @@
       <c r="C8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1089,13 +1273,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
@@ -1161,26 +1345,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1193,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAF6AF0-D333-485E-AC0B-0E3E3439BB4E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1401,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="B3" s="6"/>
     </row>
@@ -1241,6 +1425,408 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update ToDo para el JavaDoc y el diseño de pruebas
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336B56A-FCE7-4C88-8995-5D7BD2CE28ED}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C090E1-4E60-49D2-8286-EB2BD246796A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
     <sheet name="Must Have" sheetId="2" r:id="rId2"/>
     <sheet name="Entregables" sheetId="3" r:id="rId3"/>
     <sheet name="Pruebas" sheetId="4" r:id="rId4"/>
+    <sheet name="JavaDoc" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="145">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -250,9 +251,6 @@
     <t>darDecoraciones</t>
   </si>
   <si>
-    <t>agregarDecoracion</t>
-  </si>
-  <si>
     <t>crearDecoraciones</t>
   </si>
   <si>
@@ -401,13 +399,73 @@
   </si>
   <si>
     <t>agregardecoracion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonificacion </t>
+  </si>
+  <si>
+    <t>Decoración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nave </t>
+  </si>
+  <si>
+    <t>mover</t>
+  </si>
+  <si>
+    <t>dX</t>
+  </si>
+  <si>
+    <t>dY</t>
+  </si>
+  <si>
+    <t>Proyectil</t>
+  </si>
+  <si>
+    <t>SpriteMovimiento</t>
+  </si>
+  <si>
+    <t>Decoracion</t>
+  </si>
+  <si>
+    <t>NombreNoExisteException</t>
+  </si>
+  <si>
+    <t>PuntajeNoExisteException</t>
+  </si>
+  <si>
+    <t>HiloBonus</t>
+  </si>
+  <si>
+    <t>HiloInvulnerabilidad</t>
+  </si>
+  <si>
+    <t>HiloProyectil</t>
+  </si>
+  <si>
+    <t>DialogRanking</t>
+  </si>
+  <si>
+    <t>PanelDatos</t>
+  </si>
+  <si>
+    <t>PanelInicio</t>
+  </si>
+  <si>
+    <t>PanelJuego</t>
+  </si>
+  <si>
+    <t>Ventana</t>
+  </si>
+  <si>
+    <t>Camila</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,8 +485,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,8 +518,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -477,11 +548,129 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -515,11 +704,90 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1070,10 +1338,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1345,26 +1613,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1378,7 +1646,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1669,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="6"/>
     </row>
@@ -1425,7 +1693,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1435,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,382 +1719,757 @@
     <col min="6" max="6" width="5.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="24"/>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" t="s">
+      <c r="C2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="25"/>
+      <c r="H2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s">
         <v>76</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="I3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="25"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="25"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="25"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="19"/>
+      <c r="C19" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="25"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="25"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="25"/>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="25"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="19"/>
+      <c r="C35" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="19"/>
+      <c r="C36" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="25"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="19"/>
+      <c r="C37" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="25"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="21"/>
+      <c r="C38" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="25"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="19"/>
+      <c r="C40" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="25"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="19"/>
+      <c r="C41" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="25"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="19"/>
+      <c r="C42" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="25"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="21"/>
+      <c r="C43" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="25"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="25"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="25"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="19"/>
+      <c r="C47" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21"/>
+      <c r="C48" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="25"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23"/>
+      <c r="B49" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="26"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>71</v>
-      </c>
-      <c r="E5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" t="s">
-        <v>73</v>
-      </c>
-      <c r="E46" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="27"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="27"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="D2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="9"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Hecho el JavaDoc de la interfaz Movible y la clase Nave
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C31A7B-CC82-4C26-AAB0-6AE4231CBC8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0A951-EB3B-4E8E-9D5A-A3C75F5D0C1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
     <sheet name="Pruebas" sheetId="4" r:id="rId4"/>
     <sheet name="JavaDoc" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="144">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -401,12 +401,6 @@
     <t>agregardecoracion</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonificacion </t>
-  </si>
-  <si>
-    <t>Decoración</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nave </t>
   </si>
   <si>
@@ -462,16 +456,13 @@
   </si>
   <si>
     <t>Palma</t>
-  </si>
-  <si>
-    <t>camila</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +485,13 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -676,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -729,6 +727,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1619,49 +1618,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAF6AF0-D333-485E-AC0B-0E3E3439BB4E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1679,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,16 +1710,16 @@
       <c r="E1" s="16"/>
       <c r="F1" s="24"/>
       <c r="H1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>128</v>
-      </c>
-      <c r="K1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1731,7 +1734,7 @@
       <c r="E2" s="16"/>
       <c r="F2" s="25"/>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I2" t="s">
         <v>76</v>
@@ -1750,7 +1753,7 @@
       </c>
       <c r="F3" s="25"/>
       <c r="I3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2248,21 +2251,6 @@
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
       <c r="F49" s="26"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
@@ -2279,7 +2267,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,31 +2289,31 @@
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -2335,14 +2323,14 @@
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2351,35 +2339,38 @@
         <v>56</v>
       </c>
       <c r="B4" s="9"/>
+      <c r="C4" s="27" t="s">
+        <v>142</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2391,14 +2382,14 @@
         <v>20</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2407,7 +2398,7 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2415,30 +2406,40 @@
         <v>64</v>
       </c>
       <c r="B8" s="9"/>
+      <c r="C8" s="27" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C9" s="27" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B11" s="9"/>
+      <c r="C11" s="27" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2446,23 +2447,26 @@
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="27" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" s="9"/>
+      <c r="C14" s="27" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Diseño de pruebas para el método iniciarJuego
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0A951-EB3B-4E8E-9D5A-A3C75F5D0C1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5051790-7C2E-4B22-92FA-28A52E148292}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="145">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>Palma</t>
+  </si>
+  <si>
+    <t>proyectil</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -670,11 +673,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -728,11 +788,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -860,6 +925,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1682,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,6 +1771,7 @@
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1709,12 +1785,13 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="24"/>
-      <c r="H1" t="s">
+      <c r="H1" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="32" t="s">
         <v>126</v>
       </c>
+      <c r="J1" s="33"/>
       <c r="K1" t="s">
         <v>127</v>
       </c>
@@ -1733,14 +1810,18 @@
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="25"/>
-      <c r="H2" t="s">
+      <c r="H2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="20" t="s">
         <v>76</v>
       </c>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
       <c r="B3" s="15" t="s">
         <v>76</v>
       </c>
@@ -1752,9 +1833,11 @@
         <v>76</v>
       </c>
       <c r="F3" s="25"/>
-      <c r="I3" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="22" t="s">
         <v>126</v>
       </c>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
@@ -1812,129 +1895,131 @@
       <c r="E7" s="22"/>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>117</v>
+      </c>
       <c r="F8" s="25"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E11" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>117</v>
-      </c>
-      <c r="F9" s="25"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" s="25"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" s="25"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>116</v>
       </c>
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>117</v>
-      </c>
+      <c r="C15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="25"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>118</v>
+      </c>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>118</v>
-      </c>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="25"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="20" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1943,7 +2028,7 @@
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="20" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -1952,48 +2037,52 @@
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>119</v>
+      </c>
       <c r="F22" s="25"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="25"/>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="25" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>78</v>
@@ -2006,7 +2095,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>78</v>
@@ -2019,7 +2108,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>78</v>
@@ -2030,35 +2119,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="20" t="s">
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="25" t="s">
-        <v>20</v>
-      </c>
+      <c r="B29" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -2067,194 +2154,176 @@
     </row>
     <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>115</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C31" s="16"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="25"/>
     </row>
-    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
       <c r="F32" s="25"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="19"/>
+      <c r="C33" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="25"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="25"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
       <c r="C35" s="20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="25"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="21"/>
+      <c r="C36" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="25"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
+      <c r="B37" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
       <c r="F37" s="25"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="21"/>
-      <c r="C38" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="19"/>
+      <c r="C38" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="25"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
       <c r="F39" s="25"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="19"/>
       <c r="C40" s="20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="25"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="21"/>
+      <c r="C41" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
       <c r="F41" s="25"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
       <c r="F42" s="25"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
-      <c r="C43" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
+      <c r="B43" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>113</v>
+      </c>
       <c r="F43" s="25"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="15" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="19"/>
+      <c r="C45" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="25"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>113</v>
-      </c>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="25"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="21"/>
+      <c r="C46" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
       <c r="F46" s="25"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="19"/>
-      <c r="C47" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="21"/>
-      <c r="C48" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="25"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="15" t="s">
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="23"/>
+      <c r="B47" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="26"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="26"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F1048576 J1:J1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2266,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2295,6 +2364,9 @@
         <v>134</v>
       </c>
       <c r="E1" s="1"/>
+      <c r="F1" s="27" t="s">
+        <v>142</v>
+      </c>
       <c r="G1" s="1" t="s">
         <v>137</v>
       </c>
@@ -2329,6 +2401,9 @@
         <v>42</v>
       </c>
       <c r="E3" s="1"/>
+      <c r="F3" s="27" t="s">
+        <v>142</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>139</v>
       </c>
@@ -2338,7 +2413,9 @@
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C4" s="27" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
Actualizado el To Do
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5051790-7C2E-4B22-92FA-28A52E148292}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{794D0A55-5E8F-4421-A1CB-A6E7732049EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Pruebas" sheetId="4" r:id="rId4"/>
     <sheet name="JavaDoc" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="145">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -221,18 +221,9 @@
     <t>JugadorRepetidoException</t>
   </si>
   <si>
-    <t>Comparable</t>
-  </si>
-  <si>
     <t>Ver si hay pelotas vivas</t>
   </si>
   <si>
-    <t>Jframe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jpanel </t>
-  </si>
-  <si>
     <t>Bonificacion</t>
   </si>
   <si>
@@ -459,6 +450,15 @@
   </si>
   <si>
     <t>proyectil</t>
+  </si>
+  <si>
+    <t>Disparable</t>
+  </si>
+  <si>
+    <t>Insertar jugador al ranking</t>
+  </si>
+  <si>
+    <t>Javier</t>
   </si>
 </sst>
 </file>
@@ -797,7 +797,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -925,16 +925,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1452,10 +1442,10 @@
         <v>40</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>20</v>
@@ -1475,7 +1465,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
@@ -1509,7 +1499,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>58</v>
@@ -1518,7 +1508,7 @@
         <v>59</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>20</v>
@@ -1720,7 +1710,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" s="6"/>
     </row>
@@ -1736,7 +1726,7 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -1776,66 +1766,66 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="24"/>
       <c r="H1" s="31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="25"/>
       <c r="H2" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F3" s="25"/>
       <c r="H3" s="21"/>
       <c r="I3" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J3" s="30"/>
     </row>
@@ -1845,10 +1835,10 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>20</v>
@@ -1856,14 +1846,14 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>20</v>
@@ -1871,14 +1861,14 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>20</v>
@@ -1886,10 +1876,10 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -1897,16 +1887,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -1915,20 +1905,20 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -1936,16 +1926,16 @@
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1954,14 +1944,14 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F13" s="25"/>
     </row>
@@ -1969,17 +1959,17 @@
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -1989,19 +1979,19 @@
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F16" s="25"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -2010,7 +2000,7 @@
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -2019,7 +2009,7 @@
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -2028,7 +2018,7 @@
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -2037,7 +2027,7 @@
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2047,19 +2037,19 @@
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F22" s="25"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -2069,10 +2059,10 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -2082,10 +2072,10 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -2095,10 +2085,10 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -2108,10 +2098,10 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -2121,10 +2111,10 @@
     </row>
     <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -2134,10 +2124,10 @@
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -2145,7 +2135,7 @@
     </row>
     <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -2154,7 +2144,7 @@
     </row>
     <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -2163,10 +2153,10 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2175,7 +2165,7 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="19"/>
       <c r="C33" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
@@ -2184,7 +2174,7 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
       <c r="C34" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
@@ -2193,7 +2183,7 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
       <c r="C35" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
@@ -2202,7 +2192,7 @@
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="21"/>
       <c r="C36" s="22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -2210,10 +2200,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
@@ -2222,7 +2212,7 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
@@ -2231,7 +2221,7 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="19"/>
       <c r="C39" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
@@ -2240,7 +2230,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="19"/>
       <c r="C40" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
@@ -2249,7 +2239,7 @@
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="21"/>
       <c r="C41" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -2257,10 +2247,10 @@
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -2268,24 +2258,24 @@
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F43" s="25"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
@@ -2296,7 +2286,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="19"/>
       <c r="C45" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
@@ -2305,7 +2295,7 @@
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="21"/>
       <c r="C46" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
@@ -2314,7 +2304,7 @@
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="23"/>
       <c r="B47" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -2335,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,54 +2348,57 @@
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2417,65 +2410,65 @@
         <v>20</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2484,7 +2477,7 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2495,54 +2488,54 @@
         <v>20</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JavaDoc tipos de Proyectiles
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE5693E-C95F-472D-A419-360AB0CB5A06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73368DDD-4F18-4D2A-9D12-0AED62009784}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="151">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -518,7 +518,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +543,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -731,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +794,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1371,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4CC39-0340-4176-B8BF-532469A804C2}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2292,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,7 +2553,7 @@
       <c r="A19" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="25" t="s">
         <v>138</v>
       </c>
@@ -2553,7 +2562,9 @@
       <c r="A20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C20" s="25" t="s">
         <v>138</v>
       </c>
@@ -2562,7 +2573,9 @@
       <c r="A21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C21" s="25" t="s">
         <v>138</v>
       </c>
@@ -2571,7 +2584,9 @@
       <c r="A22" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C22" s="25" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
JavaDoc interfaz Disparable y clase Pelota
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73368DDD-4F18-4D2A-9D12-0AED62009784}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F227BE48-269E-460F-B7EA-578F222F8B8B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="151">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2302,7 +2302,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,7 +2475,9 @@
       <c r="A11" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="34" t="s">
+        <v>20</v>
+      </c>
       <c r="C11" s="25" t="s">
         <v>138</v>
       </c>
@@ -2544,7 +2546,9 @@
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C18" s="25" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
JavaDoc HiloBonus e HiloJuego
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F227BE48-269E-460F-B7EA-578F222F8B8B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827ADBDE-394A-4172-9FFA-4D13E4E67112}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2302,7 +2302,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2329,9 @@
       <c r="D1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="F1" s="25" t="s">
         <v>138</v>
       </c>
@@ -2371,7 +2373,9 @@
       <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="F3" s="25" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
JavaDoc HiloNave, HiloPelotas, HiloProyectil
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827ADBDE-394A-4172-9FFA-4D13E4E67112}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01787149-26EE-4F8B-8256-7BA93FEF9FBC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="151">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2302,7 +2302,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,7 +2392,9 @@
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="F4" s="25" t="s">
         <v>138</v>
       </c>
@@ -2409,7 +2411,9 @@
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="25" t="s">
         <v>138</v>
       </c>
@@ -2426,7 +2430,9 @@
       <c r="D6" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="F6" s="25" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Update ToDo y diseño de pruebas
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01787149-26EE-4F8B-8256-7BA93FEF9FBC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A87D39-7D3C-4C6B-AC73-545EF0A8086D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="153">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -395,12 +395,6 @@
     <t>mover</t>
   </si>
   <si>
-    <t>dX</t>
-  </si>
-  <si>
-    <t>dY</t>
-  </si>
-  <si>
     <t>Proyectil</t>
   </si>
   <si>
@@ -477,6 +471,18 @@
   </si>
   <si>
     <t>ProyectilRapido</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Diseñado</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -737,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -787,11 +793,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -799,11 +802,63 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -911,6 +966,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1364,10 +1429,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1428,7 +1493,7 @@
         <v>40</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>66</v>
@@ -1451,7 +1516,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
@@ -1639,26 +1704,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1712,7 +1777,7 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1723,7 +1788,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1733,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,11 +1811,12 @@
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1760,22 +1826,19 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="23"/>
-      <c r="H1" s="29" t="s">
+      <c r="F1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="I1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="15" t="s">
         <v>72</v>
@@ -1785,18 +1848,21 @@
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="24"/>
-      <c r="H2" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="20" t="s">
+      <c r="F2" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="32"/>
+      <c r="I2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="27"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="34"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>73</v>
@@ -1808,14 +1874,17 @@
       <c r="E3" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="F3" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="J3" s="28"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="35"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>63</v>
       </c>
@@ -1829,8 +1898,9 @@
       <c r="F4" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>74</v>
       </c>
@@ -1844,8 +1914,9 @@
       <c r="F5" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>76</v>
       </c>
@@ -1859,8 +1930,15 @@
       <c r="F6" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="32"/>
+      <c r="J6" t="s">
+        <v>150</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
         <v>78</v>
       </c>
@@ -1870,8 +1948,15 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
       <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G7" s="32"/>
+      <c r="J7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>77</v>
       </c>
@@ -1885,8 +1970,9 @@
         <v>113</v>
       </c>
       <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -1894,8 +1980,9 @@
         <v>112</v>
       </c>
       <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>80</v>
       </c>
@@ -1907,8 +1994,9 @@
         <v>112</v>
       </c>
       <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22" t="s">
@@ -1918,8 +2006,9 @@
         <v>116</v>
       </c>
       <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>81</v>
       </c>
@@ -1927,8 +2016,9 @@
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>90</v>
       </c>
@@ -1940,8 +2030,9 @@
         <v>112</v>
       </c>
       <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20" t="s">
@@ -1951,8 +2042,9 @@
         <v>113</v>
       </c>
       <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="20" t="s">
         <v>89</v>
@@ -1960,8 +2052,9 @@
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="24"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22" t="s">
@@ -1971,8 +2064,9 @@
         <v>114</v>
       </c>
       <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="32"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>82</v>
       </c>
@@ -1982,8 +2076,9 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="24"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="32"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="20" t="s">
         <v>90</v>
@@ -1991,8 +2086,9 @@
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="32"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="20" t="s">
         <v>77</v>
@@ -2000,8 +2096,9 @@
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="24"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="32"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="20" t="s">
         <v>81</v>
@@ -2009,8 +2106,9 @@
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
         <v>78</v>
@@ -2018,8 +2116,9 @@
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="32"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22" t="s">
@@ -2029,8 +2128,9 @@
         <v>115</v>
       </c>
       <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="32"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>83</v>
       </c>
@@ -2042,8 +2142,9 @@
       <c r="F23" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="32"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
         <v>84</v>
       </c>
@@ -2055,8 +2156,9 @@
       <c r="F24" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="32"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>85</v>
       </c>
@@ -2068,8 +2170,9 @@
       <c r="F25" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="32"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>86</v>
       </c>
@@ -2081,8 +2184,9 @@
       <c r="F26" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="32"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>87</v>
       </c>
@@ -2094,8 +2198,9 @@
       <c r="F27" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="32"/>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
         <v>88</v>
       </c>
@@ -2107,8 +2212,9 @@
       <c r="F28" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="32"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="s">
         <v>91</v>
       </c>
@@ -2118,8 +2224,9 @@
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="24"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="32"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
         <v>92</v>
       </c>
@@ -2127,8 +2234,9 @@
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="24"/>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="32"/>
+    </row>
+    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
         <v>93</v>
       </c>
@@ -2136,8 +2244,9 @@
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="24"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="32"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
         <v>99</v>
       </c>
@@ -2147,8 +2256,9 @@
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="24"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="32"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="19"/>
       <c r="C33" s="20" t="s">
         <v>95</v>
@@ -2156,8 +2266,9 @@
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="32"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
       <c r="C34" s="20" t="s">
         <v>96</v>
@@ -2165,8 +2276,9 @@
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="24"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="32"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
       <c r="C35" s="20" t="s">
         <v>97</v>
@@ -2174,8 +2286,9 @@
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="24"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="32"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="21"/>
       <c r="C36" s="22" t="s">
         <v>98</v>
@@ -2183,8 +2296,9 @@
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="32"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
         <v>105</v>
       </c>
@@ -2194,8 +2308,9 @@
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
       <c r="F37" s="24"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="32"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38" s="20" t="s">
         <v>101</v>
@@ -2203,8 +2318,9 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
       <c r="F38" s="24"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="32"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="19"/>
       <c r="C39" s="20" t="s">
         <v>102</v>
@@ -2212,8 +2328,9 @@
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="24"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="32"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="19"/>
       <c r="C40" s="20" t="s">
         <v>103</v>
@@ -2221,8 +2338,9 @@
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="32"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="21"/>
       <c r="C41" s="22" t="s">
         <v>104</v>
@@ -2230,8 +2348,9 @@
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
       <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="32"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
         <v>106</v>
       </c>
@@ -2240,9 +2359,12 @@
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" s="32"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="s">
         <v>107</v>
       </c>
@@ -2253,10 +2375,13 @@
       <c r="E43" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="F43" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G43" s="32"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
       <c r="B44" s="17" t="s">
         <v>109</v>
       </c>
@@ -2268,29 +2393,46 @@
       <c r="F44" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="32"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="19"/>
       <c r="C45" s="20" t="s">
         <v>106</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
-      <c r="F45" s="24"/>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="32"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="21"/>
       <c r="C46" s="22" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
-      <c r="F46" s="24"/>
+      <c r="F46" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" s="32"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576 J1:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="F1:G1048576 K1:K1048576">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"d"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2302,7 +2444,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,57 +2460,66 @@
     <col min="9" max="9" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C1" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>141</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>42</v>
@@ -2377,16 +2528,16 @@
         <v>20</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="1" t="s">
@@ -2396,16 +2547,19 @@
         <v>20</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" s="9"/>
       <c r="D5" s="1" t="s">
@@ -2415,51 +2569,54 @@
         <v>20</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B6" s="9"/>
       <c r="D6" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G6" s="20"/>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="9"/>
       <c r="D7" s="20"/>
-      <c r="E7" s="33"/>
+      <c r="E7" s="30"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B8" s="9"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="33"/>
+      <c r="E8" s="30"/>
       <c r="G8" s="20"/>
-      <c r="H8" s="33"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -2467,32 +2624,34 @@
         <v>20</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="9"/>
+        <v>125</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -2500,28 +2659,28 @@
         <v>20</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -2529,10 +2688,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -2540,16 +2699,16 @@
         <v>20</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2560,63 +2719,63 @@
         <v>20</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="34"/>
+        <v>123</v>
+      </c>
+      <c r="B19" s="31"/>
       <c r="C19" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576 E13:E1048576 E1:E8 H12:H1048576 H1:H8">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Diseño de pruebas métodos de la clase Pelotas
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A87D39-7D3C-4C6B-AC73-545EF0A8086D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE86DC0-B439-445D-954F-45E28E1A91CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="153">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -556,7 +556,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -739,11 +739,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -814,31 +838,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -861,11 +871,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -966,16 +976,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1429,10 +1429,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1704,26 +1704,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1788,7 +1788,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1798,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,7 +1947,9 @@
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>149</v>
+      </c>
       <c r="G7" s="32"/>
       <c r="J7" t="s">
         <v>151</v>
@@ -1960,138 +1962,142 @@
       <c r="B8" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>79</v>
-      </c>
+      <c r="C8" s="18"/>
       <c r="D8" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="36" t="s">
+        <v>149</v>
+      </c>
       <c r="G8" s="32"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="36" t="s">
+        <v>149</v>
+      </c>
       <c r="G9" s="32"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E11" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="32"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>116</v>
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>112</v>
-      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="24"/>
       <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20" t="s">
+      <c r="B14" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>113</v>
+      <c r="E14" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>113</v>
+      </c>
       <c r="F15" s="24"/>
       <c r="G15" s="32"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>114</v>
-      </c>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="24"/>
       <c r="G16" s="32"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>114</v>
+      </c>
       <c r="F17" s="24"/>
       <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="24"/>
       <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="20" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -2101,7 +2107,7 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -2111,48 +2117,46 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="24"/>
       <c r="G21" s="32"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>115</v>
-      </c>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="24"/>
       <c r="G22" s="32"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="32"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="32"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="24" t="s">
         <v>20</v>
       </c>
@@ -2160,7 +2164,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>75</v>
@@ -2174,7 +2178,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>75</v>
@@ -2188,7 +2192,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>75</v>
@@ -2200,45 +2204,51 @@
       </c>
       <c r="G27" s="32"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="21" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="32"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C29" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="24"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="24" t="s">
+        <v>20</v>
+      </c>
       <c r="G29" s="32"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="16"/>
+        <v>91</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>111</v>
+      </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="24"/>
+      <c r="F30" s="24" t="s">
+        <v>149</v>
+      </c>
       <c r="G30" s="32"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -2246,32 +2256,32 @@
       <c r="F31" s="24"/>
       <c r="G31" s="32"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="24"/>
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="B33" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
       <c r="F33" s="24"/>
       <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
       <c r="C34" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
@@ -2281,49 +2291,49 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
       <c r="C35" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="24"/>
       <c r="G35" s="32"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="21"/>
-      <c r="C36" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="19"/>
+      <c r="C36" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="24"/>
       <c r="G36" s="32"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="21"/>
+      <c r="C37" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
       <c r="F37" s="24"/>
       <c r="G37" s="32"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
+      <c r="B38" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
       <c r="F38" s="24"/>
       <c r="G38" s="32"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="19"/>
       <c r="C39" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
@@ -2333,105 +2343,115 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="19"/>
       <c r="C40" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="24"/>
       <c r="G40" s="32"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="21"/>
-      <c r="C41" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="19"/>
+      <c r="C41" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
       <c r="F41" s="24"/>
       <c r="G41" s="32"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="24" t="s">
-        <v>149</v>
-      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="24"/>
       <c r="G42" s="32"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>110</v>
-      </c>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
       <c r="F43" s="24" t="s">
         <v>149</v>
       </c>
       <c r="G43" s="32"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="17" t="s">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" s="32"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="29"/>
+      <c r="B45" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C45" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" s="32"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="20" t="s">
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="32"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="19"/>
+      <c r="C46" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="G45" s="32"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
-      <c r="C46" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="24" t="s">
         <v>149</v>
       </c>
       <c r="G46" s="32"/>
     </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="21"/>
+      <c r="C47" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" s="32"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F1:G1048576 K1:K1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2443,7 +2463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2775,7 +2795,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576 E13:E1048576 E1:E8 H12:H1048576 H1:H8">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
JavaDoc Proyectil y update ToDo
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE86DC0-B439-445D-954F-45E28E1A91CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3FEC17-BCB9-4EAC-AA78-5A5C069DA6DB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimientos" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="153">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -1800,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E10994E-EDA9-456C-8C8D-BB11D045C9D0}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -2463,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2559,7 +2559,12 @@
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
@@ -2581,7 +2586,12 @@
       <c r="A5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
@@ -2603,7 +2613,12 @@
       <c r="A6" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>130</v>
       </c>
@@ -2620,7 +2635,12 @@
       <c r="A7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="D7" s="20"/>
       <c r="E7" s="30"/>
       <c r="G7" s="20"/>
@@ -2630,7 +2650,12 @@
       <c r="A8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="D8" s="20"/>
       <c r="E8" s="30"/>
       <c r="G8" s="20"/>
@@ -2686,7 +2711,9 @@
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="25" t="s">
         <v>137</v>
       </c>
@@ -2695,7 +2722,9 @@
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="25" t="s">
         <v>137</v>
       </c>
@@ -2726,7 +2755,9 @@
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B17" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C17" s="25" t="s">
         <v>137</v>
       </c>
@@ -2746,7 +2777,9 @@
       <c r="A19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="C19" s="25" t="s">
         <v>136</v>
       </c>
@@ -2788,7 +2821,9 @@
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C23" s="25" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
JavaDoc Ventana, todo el JavaDoc ha sido realizado
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F56F5E-DCB3-4938-A363-1DA20E2B5399}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F748E8B-C994-49A3-B480-FBA6B2C83652}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="152">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -1261,7 +1261,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="2" max="2" width="4" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +1734,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,7 +2461,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,7 +2557,9 @@
       <c r="G3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I3" s="25" t="s">
         <v>135</v>
       </c>
@@ -2584,7 +2586,9 @@
       <c r="G4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I4" s="25" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
Update ToDo para diseño de pruebas unit.
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F748E8B-C994-49A3-B480-FBA6B2C83652}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B282E8-0D22-4013-AEDF-34E53A83E195}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,8 @@
     <sheet name="Must Have" sheetId="2" r:id="rId2"/>
     <sheet name="Entregables" sheetId="3" r:id="rId3"/>
     <sheet name="Pruebas" sheetId="4" r:id="rId4"/>
-    <sheet name="JavaDoc" sheetId="5" r:id="rId5"/>
+    <sheet name="PruebasUnit" sheetId="6" r:id="rId5"/>
+    <sheet name="JavaDoc" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="182">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -480,6 +481,96 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Prueba para verificar la imagen dada</t>
+  </si>
+  <si>
+    <t>aArrayList</t>
+  </si>
+  <si>
+    <t>Se prueba con el método de Juego getBonus</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>setSiguiente</t>
+  </si>
+  <si>
+    <t>getSiguiente</t>
+  </si>
+  <si>
+    <t>setAnterior</t>
+  </si>
+  <si>
+    <t>getAnterior</t>
+  </si>
+  <si>
+    <t>getHitBox</t>
+  </si>
+  <si>
+    <t>Subclases</t>
+  </si>
+  <si>
+    <t>Prueba a realizar</t>
+  </si>
+  <si>
+    <t>Pruebas secundarias (pueden ser parte Escenario)</t>
+  </si>
+  <si>
+    <t>disminuirVida</t>
+  </si>
+  <si>
+    <t>esHoja</t>
+  </si>
+  <si>
+    <t>crearArreglo</t>
+  </si>
+  <si>
+    <t>Se prueba con el método de Juego getPelotas</t>
+  </si>
+  <si>
+    <t>hayVivas</t>
+  </si>
+  <si>
+    <t>darPeso</t>
+  </si>
+  <si>
+    <t>Depende de si es una pelota o un bonus</t>
+  </si>
+  <si>
+    <t>Se prueba en el proyectil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAN SIDO IMPLEMENTADAS EN LA CLASE JUEGO. </t>
+  </si>
+  <si>
+    <t>Prueba imagen, velocidad y daño dado</t>
+  </si>
+  <si>
+    <t>agregarDecoracion</t>
+  </si>
+  <si>
+    <t>guardarPelotas</t>
+  </si>
+  <si>
+    <t>guardarPartida y cargarPartida</t>
+  </si>
+  <si>
+    <t>localizarUltimoBonus</t>
+  </si>
+  <si>
+    <t>METODOS ORDENAR DISEÑADOS E IMPLEMENTADOS</t>
+  </si>
+  <si>
+    <t>METODOS BUSCAR DISEÑADOS E IMPLEMENTADOS</t>
   </si>
 </sst>
 </file>
@@ -521,7 +612,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -552,8 +643,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -760,11 +899,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -778,12 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -841,11 +1044,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1426,10 +1715,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B20">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1464,15 +1753,15 @@
       <c r="B1" s="1">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1483,19 +1772,19 @@
       <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1506,17 +1795,17 @@
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1527,15 +1816,15 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1546,19 +1835,19 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1569,13 +1858,13 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1586,19 +1875,19 @@
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1609,15 +1898,15 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1628,17 +1917,17 @@
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1649,19 +1938,19 @@
       <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1672,13 +1961,13 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1689,38 +1978,38 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1734,46 +2023,46 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="26"/>
+    <col min="2" max="2" width="2.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="38"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="38"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="24" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1781,11 +2070,13 @@
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="38" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1808,7 +2099,7 @@
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.140625" style="13" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" style="11" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.42578125" style="5" customWidth="1"/>
   </cols>
@@ -1817,117 +2108,117 @@
       <c r="A1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="23" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="I1" s="27" t="s">
+      <c r="G1" s="30"/>
+      <c r="I1" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="K1" s="33"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="24" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="I2" s="19" t="s">
+      <c r="G2" s="30"/>
+      <c r="I2" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="34"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22" t="s">
+      <c r="G3" s="30"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="K3" s="35"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="32"/>
+      <c r="F4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="32"/>
+      <c r="F5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="32"/>
+      <c r="F6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="30"/>
       <c r="J6" t="s">
         <v>149</v>
       </c>
@@ -1936,18 +2227,18 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="24" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="30"/>
       <c r="J7" t="s">
         <v>150</v>
       </c>
@@ -1956,499 +2247,499 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="38" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="32"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="32"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="32"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="32"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="32"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="32"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="32"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="32"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="32"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="30"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="32"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="32"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="32"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="32"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="32"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="32"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="30"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="32"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="32"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="30"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="32"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="24" t="s">
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="30"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="32"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="32"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="32"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="32"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="30"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="32"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="30"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="32"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="21"/>
-      <c r="C37" s="22" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="32"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="32"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="20" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="32"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="20" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="32"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="20" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="32"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="21"/>
-      <c r="C42" s="22" t="s">
+      <c r="B42" s="19"/>
+      <c r="C42" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="32"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="30"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="24" t="s">
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G43" s="32"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16" t="s">
+      <c r="C44" s="14"/>
+      <c r="D44" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G44" s="32"/>
+      <c r="G44" s="30"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="27"/>
+      <c r="B45" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="32"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
-      <c r="C46" s="20" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="24" t="s">
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G46" s="32"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="21"/>
-      <c r="C47" s="22" t="s">
+      <c r="B47" s="19"/>
+      <c r="C47" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="24" t="s">
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G47" s="32"/>
+      <c r="G47" s="30"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:G1048576 K1:K1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2457,10 +2748,659 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="58"/>
+      <c r="B3" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="54"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="69"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="54"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="69"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="68"/>
+      <c r="F7" s="69"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="68"/>
+      <c r="F9" s="69"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="65"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="69"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="59"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" s="60"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="71"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="58"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="65"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="69"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="68"/>
+      <c r="F16" s="69"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="65"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="58"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="65"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="58"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="69"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="59"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="61"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="73"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="63"/>
+      <c r="C23" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="E23" s="70"/>
+      <c r="F23" s="71"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="65"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="69"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="59"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="60"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="58"/>
+      <c r="B29" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="54"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="69"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="58"/>
+      <c r="B30" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="54"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="69"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="58"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="65"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="69"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="58"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="65"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="69"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="58"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="65"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="69"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="59"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="72"/>
+      <c r="F34" s="73"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="63"/>
+      <c r="C35" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="70"/>
+      <c r="F35" s="71"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="58"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="65"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="69"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="58"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="65"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="69"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="58"/>
+      <c r="B38" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="68"/>
+      <c r="F38" s="69"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="58"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="68"/>
+      <c r="F39" s="69"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="58"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="68"/>
+      <c r="F40" s="69"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="58"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="68"/>
+      <c r="F41" s="69"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="58"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="68"/>
+      <c r="F42" s="69"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="58"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="68"/>
+      <c r="F43" s="69"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="58"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="65"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="69"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="58"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="65"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="69"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="58"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="65"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="69"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="58"/>
+      <c r="B47" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="58"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="65"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="69"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="58"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="65"/>
+      <c r="E49" s="68"/>
+      <c r="F49" s="69"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="58"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="65"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="58"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="65"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="69"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="58"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="65"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="69"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="59"/>
+      <c r="B53" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B27:D27"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E1:F1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1245BB-0F59-435D-BB6C-DA4E4604C171}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -2468,41 +3408,41 @@
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="25"/>
+    <col min="3" max="3" width="11.42578125" style="23"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="25"/>
+    <col min="6" max="6" width="11.42578125" style="23"/>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="25"/>
+    <col min="9" max="9" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2510,28 +3450,28 @@
       <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>138</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="25" t="s">
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2539,28 +3479,28 @@
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="25" t="s">
+      <c r="H3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2568,28 +3508,28 @@
       <c r="A4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>136</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2597,19 +3537,19 @@
       <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="25" t="s">
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2617,75 +3557,75 @@
       <c r="A6" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>136</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="30"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="30"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="30"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="28"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="30"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="30"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="28"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="30"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2693,10 +3633,10 @@
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2704,10 +3644,10 @@
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2715,10 +3655,10 @@
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2726,10 +3666,10 @@
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2737,10 +3677,10 @@
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2748,10 +3688,10 @@
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2759,10 +3699,10 @@
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="25" t="s">
+      <c r="B17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2770,10 +3710,10 @@
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2781,10 +3721,10 @@
       <c r="A19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="25" t="s">
+      <c r="B19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2792,10 +3732,10 @@
       <c r="A20" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="25" t="s">
+      <c r="B20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2803,10 +3743,10 @@
       <c r="A21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="25" t="s">
+      <c r="B21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2814,10 +3754,10 @@
       <c r="A22" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="25" t="s">
+      <c r="B22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2825,10 +3765,10 @@
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="25" t="s">
+      <c r="B23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diseño de pruebas para clases Bonificacion y Decoracion
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B282E8-0D22-4013-AEDF-34E53A83E195}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE3930E-ADF7-46A0-BEF2-74C47EE24412}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="184">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -571,6 +571,12 @@
   </si>
   <si>
     <t>METODOS BUSCAR DISEÑADOS E IMPLEMENTADOS</t>
+  </si>
+  <si>
+    <t>getBonus</t>
+  </si>
+  <si>
+    <t>CrearBonus</t>
   </si>
 </sst>
 </file>
@@ -973,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,22 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1084,9 +1075,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1099,9 +1087,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1119,6 +1104,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2749,10 +2758,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,320 +2773,346 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="47" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="69"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="56" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="56" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="62"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="56" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="62"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="53" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="E7" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="62"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="53" t="s">
+      <c r="A8" s="52"/>
+      <c r="B8" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="62"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="53" t="s">
+      <c r="A9" s="52"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
+      <c r="E9" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="62"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="53" t="s">
+      <c r="A10" s="52"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="69"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="62"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="55" t="s">
+      <c r="A11" s="53"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="66"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="62" t="s">
+      <c r="B12" s="57"/>
+      <c r="C12" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
+      <c r="E12" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="55" t="s">
+      <c r="A13" s="53"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
+      <c r="E13" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="66"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="62" t="s">
+      <c r="B14" s="57"/>
+      <c r="C14" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="71"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="53" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="69"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="53" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="D16" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="69"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="62"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="53" t="s">
+      <c r="A17" s="52"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="53" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="62"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="53" t="s">
+      <c r="A19" s="52"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="62"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="53" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="65"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="69"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="53" t="s">
+      <c r="A21" s="52"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="E21" s="68"/>
-      <c r="F21" s="69"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="62"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="59"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="55" t="s">
+      <c r="A22" s="53"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="73"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="62" t="s">
+      <c r="B23" s="57"/>
+      <c r="C23" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="E23" s="70"/>
-      <c r="F23" s="71"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="53" t="s">
+      <c r="A24" s="52"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="69"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="62"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="53" t="s">
+      <c r="A25" s="52"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="E25" s="68"/>
-      <c r="F25" s="69"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="62"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="59"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="55" t="s">
+      <c r="A26" s="53"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="D26" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="F26" s="73"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="73"/>
       <c r="E27" s="40" t="s">
         <v>20</v>
       </c>
@@ -3086,305 +3121,326 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="68" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="60"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="71"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="58"/>
-      <c r="B29" s="56" t="s">
+      <c r="A29" s="52"/>
+      <c r="B29" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="69"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="62"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="58"/>
-      <c r="B30" s="56" t="s">
+      <c r="A30" s="52"/>
+      <c r="B30" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="69"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="62"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="58"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="53" t="s">
+      <c r="A31" s="52"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="69"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="62"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="58"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="53" t="s">
+      <c r="A32" s="52"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="65"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="69"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="62"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="58"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="53" t="s">
+      <c r="A33" s="52"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="65"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="69"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="62"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="59"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="55" t="s">
+      <c r="A34" s="53"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="E34" s="72"/>
-      <c r="F34" s="73"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="63"/>
-      <c r="C35" s="62" t="s">
+      <c r="B35" s="57"/>
+      <c r="C35" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="E35" s="70"/>
-      <c r="F35" s="71"/>
+      <c r="E35" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="64"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="58"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="53" t="s">
+      <c r="A36" s="52"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="69"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="62"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="53" t="s">
+      <c r="A37" s="52"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="62"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="52"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="59"/>
+      <c r="E38" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="62"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="52"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="65"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="69"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
-      <c r="B38" s="43" t="s">
+      <c r="D39" s="59"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="62"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="52"/>
+      <c r="B40" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C40" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D40" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="68"/>
-      <c r="F38" s="69"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="58"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="44" t="s">
+      <c r="E40" s="61"/>
+      <c r="F40" s="62"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="52"/>
+      <c r="B41" s="69"/>
+      <c r="C41" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="44" t="s">
+      <c r="D41" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="68"/>
-      <c r="F39" s="69"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="58"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="44" t="s">
+      <c r="E41" s="61"/>
+      <c r="F41" s="62"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="52"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D42" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="68"/>
-      <c r="F40" s="69"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="44" t="s">
+      <c r="E42" s="61"/>
+      <c r="F42" s="62"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="52"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="44" t="s">
+      <c r="D43" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E41" s="68"/>
-      <c r="F41" s="69"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="58"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44" t="s">
+      <c r="E43" s="61"/>
+      <c r="F43" s="62"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="52"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="44" t="s">
+      <c r="D44" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="68"/>
-      <c r="F42" s="69"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="58"/>
-      <c r="B43" s="56"/>
-      <c r="C43" s="53" t="s">
+      <c r="E44" s="61"/>
+      <c r="F44" s="62"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="52"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="65" t="s">
+      <c r="D45" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="68"/>
-      <c r="F43" s="69"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="58"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="53" t="s">
-        <v>179</v>
-      </c>
-      <c r="D44" s="65"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="69"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="58"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="53" t="s">
+      <c r="E45" s="61"/>
+      <c r="F45" s="62"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="52"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="69"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="58"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="53" t="s">
+      <c r="D46" s="59"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="62"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="52"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="69"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="58"/>
-      <c r="B47" s="45" t="s">
+      <c r="D47" s="59"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="62"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="52"/>
+      <c r="B48" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="58"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="53" t="s">
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="52"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="65"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="69"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="58"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="53" t="s">
+      <c r="D49" s="59"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="62"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="52"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="65"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="69"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="58"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="53" t="s">
+      <c r="D50" s="59"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="62"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="52"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="65"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="69"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="58"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="53" t="s">
+      <c r="D51" s="59"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="62"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="52"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="65"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="69"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="58"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="53" t="s">
+      <c r="D52" s="59"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="62"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="52"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="65"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="69"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="59"/>
-      <c r="B53" s="46" t="s">
+      <c r="D53" s="59"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="62"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="53"/>
+      <c r="B54" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="33" t="s">
+      <c r="C54" s="71"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="33" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B54:D54"/>
     <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:F1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
Diseño de pruebas clase Pelota
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE3930E-ADF7-46A0-BEF2-74C47EE24412}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25E5441-37EB-4140-8818-012B42BBE30C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="183">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -526,9 +526,6 @@
   </si>
   <si>
     <t>disminuirVida</t>
-  </si>
-  <si>
-    <t>esHoja</t>
   </si>
   <si>
     <t>crearArreglo</t>
@@ -2758,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,7 +2870,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="48" t="s">
         <v>159</v>
@@ -2965,179 +2962,195 @@
         <v>166</v>
       </c>
       <c r="D14" s="54"/>
-      <c r="E14" s="63"/>
+      <c r="E14" s="63" t="s">
+        <v>20</v>
+      </c>
       <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
       <c r="B15" s="50"/>
       <c r="C15" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="61"/>
+        <v>116</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F15" s="62"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
       <c r="B16" s="50"/>
       <c r="C16" s="48" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
       <c r="D16" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="61"/>
+        <v>168</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F16" s="62"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
       <c r="B17" s="50"/>
       <c r="C17" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="D17" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="61"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
       <c r="B18" s="50"/>
       <c r="C18" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="61"/>
+      <c r="E18" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F18" s="62"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
       <c r="B19" s="50"/>
       <c r="C19" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="E19" s="61"/>
+        <v>112</v>
+      </c>
+      <c r="D19" s="59"/>
+      <c r="E19" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="62"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="52"/>
       <c r="B20" s="50"/>
       <c r="C20" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="62"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="53"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="55"/>
+      <c r="E21" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="66"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="57"/>
+      <c r="C22" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="62"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="49" t="s">
+      <c r="D22" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="52"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="64"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="62"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="52"/>
       <c r="B24" s="50"/>
       <c r="C24" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="59"/>
+        <v>113</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>162</v>
+      </c>
       <c r="E24" s="61"/>
       <c r="F24" s="62"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="61"/>
-      <c r="F25" s="62"/>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="53"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="65"/>
+      <c r="F25" s="66"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="53"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="55" t="s">
+      <c r="A26" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="72" t="s">
         <v>173</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="72" t="s">
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="D27" s="54"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="68" t="s">
-        <v>175</v>
-      </c>
-      <c r="D28" s="54"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="64"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="67"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="62"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="52"/>
       <c r="B29" s="50" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C29" s="67"/>
       <c r="D29" s="59"/>
@@ -3146,10 +3159,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="52"/>
-      <c r="B30" s="50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C30" s="67"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="48" t="s">
+        <v>73</v>
+      </c>
       <c r="D30" s="59"/>
       <c r="E30" s="61"/>
       <c r="F30" s="62"/>
@@ -3158,7 +3171,7 @@
       <c r="A31" s="52"/>
       <c r="B31" s="50"/>
       <c r="C31" s="48" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="61"/>
@@ -3168,57 +3181,61 @@
       <c r="A32" s="52"/>
       <c r="B32" s="50"/>
       <c r="C32" s="48" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="61"/>
       <c r="F32" s="62"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="59"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="62"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="53"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="49" t="s">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="53"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="55" t="s">
+      <c r="D33" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="66"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="57"/>
+      <c r="C34" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="64"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="54" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="64"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="59"/>
+      <c r="E35" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="62"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
       <c r="B36" s="50"/>
       <c r="C36" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="59"/>
+        <v>91</v>
+      </c>
+      <c r="D36" s="59" t="s">
+        <v>178</v>
+      </c>
       <c r="E36" s="61" t="s">
         <v>20</v>
       </c>
@@ -3228,11 +3245,9 @@
       <c r="A37" s="52"/>
       <c r="B37" s="50"/>
       <c r="C37" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="59" t="s">
-        <v>179</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="D37" s="59"/>
       <c r="E37" s="61" t="s">
         <v>20</v>
       </c>
@@ -3242,34 +3257,34 @@
       <c r="A38" s="52"/>
       <c r="B38" s="50"/>
       <c r="C38" s="48" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="D38" s="59"/>
-      <c r="E38" s="61" t="s">
-        <v>20</v>
-      </c>
+      <c r="E38" s="61"/>
       <c r="F38" s="62"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="59"/>
+      <c r="B39" s="69" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>95</v>
+      </c>
       <c r="E39" s="61"/>
       <c r="F39" s="62"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="52"/>
-      <c r="B40" s="69" t="s">
-        <v>178</v>
-      </c>
+      <c r="B40" s="69"/>
       <c r="C40" s="43" t="s">
-        <v>103</v>
+        <v>176</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E40" s="61"/>
       <c r="F40" s="62"/>
@@ -3278,10 +3293,10 @@
       <c r="A41" s="52"/>
       <c r="B41" s="69"/>
       <c r="C41" s="43" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41" s="61"/>
       <c r="F41" s="62"/>
@@ -3290,10 +3305,10 @@
       <c r="A42" s="52"/>
       <c r="B42" s="69"/>
       <c r="C42" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E42" s="61"/>
       <c r="F42" s="62"/>
@@ -3302,22 +3317,22 @@
       <c r="A43" s="52"/>
       <c r="B43" s="69"/>
       <c r="C43" s="43" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E43" s="61"/>
       <c r="F43" s="62"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="52"/>
-      <c r="B44" s="69"/>
-      <c r="C44" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" s="43" t="s">
-        <v>94</v>
+      <c r="B44" s="50"/>
+      <c r="C44" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="59" t="s">
+        <v>92</v>
       </c>
       <c r="E44" s="61"/>
       <c r="F44" s="62"/>
@@ -3326,11 +3341,9 @@
       <c r="A45" s="52"/>
       <c r="B45" s="50"/>
       <c r="C45" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="59" t="s">
-        <v>92</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D45" s="59"/>
       <c r="E45" s="61"/>
       <c r="F45" s="62"/>
     </row>
@@ -3338,7 +3351,7 @@
       <c r="A46" s="52"/>
       <c r="B46" s="50"/>
       <c r="C46" s="48" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="61"/>
@@ -3346,33 +3359,33 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="52"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47" s="59"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="62"/>
+      <c r="B47" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="52"/>
-      <c r="B48" s="70" t="s">
-        <v>180</v>
-      </c>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>20</v>
-      </c>
+      <c r="B48" s="50"/>
+      <c r="C48" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="59"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="62"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="52"/>
       <c r="B49" s="50"/>
       <c r="C49" s="48" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="61"/>
@@ -3382,7 +3395,7 @@
       <c r="A50" s="52"/>
       <c r="B50" s="50"/>
       <c r="C50" s="48" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="61"/>
@@ -3392,7 +3405,7 @@
       <c r="A51" s="52"/>
       <c r="B51" s="50"/>
       <c r="C51" s="48" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D51" s="59"/>
       <c r="E51" s="61"/>
@@ -3402,44 +3415,34 @@
       <c r="A52" s="52"/>
       <c r="B52" s="50"/>
       <c r="C52" s="48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D52" s="59"/>
       <c r="E52" s="61"/>
       <c r="F52" s="62"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="52"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D53" s="59"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="62"/>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="53"/>
-      <c r="B54" s="71" t="s">
-        <v>181</v>
-      </c>
-      <c r="C54" s="71"/>
-      <c r="D54" s="71"/>
-      <c r="E54" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="33" t="s">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="53"/>
+      <c r="B53" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="33" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B8:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:F1048576">

</xml_diff>

<commit_message>
Diseño de pruebas Nave, Proyectily actualizado el src para manejar los serializables y archivos de texto en las pruebas
Update JavaDoc como consecuencia de cambiar el parámetro de los métodos de recuperación, serialización y manejo de archivos de texto
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25E5441-37EB-4140-8818-012B42BBE30C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D060690-6F7B-411A-83EC-A52731E69B50}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="192">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -574,6 +574,33 @@
   </si>
   <si>
     <t>CrearBonus</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>difx</t>
+  </si>
+  <si>
+    <t>dify</t>
+  </si>
+  <si>
+    <t>hip</t>
+  </si>
+  <si>
+    <t>prop</t>
+  </si>
+  <si>
+    <t>dx</t>
+  </si>
+  <si>
+    <t>dy</t>
   </si>
 </sst>
 </file>
@@ -2755,10 +2782,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E33"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,9 +2794,10 @@
     <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.42578125" style="5"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>152</v>
       </c>
@@ -2788,8 +2816,14 @@
       <c r="F1" s="47" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>66</v>
       </c>
@@ -2804,8 +2838,14 @@
         <v>20</v>
       </c>
       <c r="F2" s="62"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="50" t="s">
         <v>140</v>
@@ -2816,8 +2856,14 @@
         <v>20</v>
       </c>
       <c r="F3" s="62"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="50" t="s">
         <v>141</v>
@@ -2828,8 +2874,14 @@
         <v>20</v>
       </c>
       <c r="F4" s="62"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="50" t="s">
         <v>142</v>
@@ -2841,7 +2893,7 @@
       </c>
       <c r="F5" s="62"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="50" t="s">
         <v>143</v>
@@ -2852,8 +2904,15 @@
         <v>20</v>
       </c>
       <c r="F6" s="62"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6">
+        <f>I3-I1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="50"/>
       <c r="C7" s="48" t="s">
@@ -2866,8 +2925,15 @@
         <v>20</v>
       </c>
       <c r="F7" s="62"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7">
+        <f>I4-I2</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="74" t="s">
         <v>182</v>
@@ -2883,7 +2949,7 @@
       </c>
       <c r="F8" s="62"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="74"/>
       <c r="C9" s="48" t="s">
@@ -2896,8 +2962,15 @@
         <v>20</v>
       </c>
       <c r="F9" s="62"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I9">
+        <f>SQRT(I6*I6+I7*I7)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
       <c r="B10" s="50"/>
       <c r="C10" s="48" t="s">
@@ -2908,8 +2981,15 @@
         <v>20</v>
       </c>
       <c r="F10" s="62"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I10">
+        <f>20/I9</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="53"/>
       <c r="B11" s="51"/>
       <c r="C11" s="49" t="s">
@@ -2923,7 +3003,7 @@
       </c>
       <c r="F11" s="66"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>125</v>
       </c>
@@ -2938,8 +3018,15 @@
         <v>20</v>
       </c>
       <c r="F12" s="64"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12">
+        <f>I10*(I3-I1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53"/>
       <c r="B13" s="51"/>
       <c r="C13" s="49" t="s">
@@ -2952,8 +3039,15 @@
         <v>20</v>
       </c>
       <c r="F13" s="66"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>191</v>
+      </c>
+      <c r="I13">
+        <f>I10*(I4-I2)</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>70</v>
       </c>
@@ -2967,7 +3061,7 @@
       </c>
       <c r="F14" s="64"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
       <c r="B15" s="50"/>
       <c r="C15" s="48" t="s">
@@ -2981,7 +3075,7 @@
       </c>
       <c r="F15" s="62"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
       <c r="B16" s="50"/>
       <c r="C16" s="48" t="s">
@@ -3070,7 +3164,9 @@
       <c r="D22" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="E22" s="63"/>
+      <c r="E22" s="63" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="64"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3176,9 @@
         <v>122</v>
       </c>
       <c r="D23" s="59"/>
-      <c r="E23" s="61"/>
+      <c r="E23" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F23" s="62"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3092,7 +3190,9 @@
       <c r="D24" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="61"/>
+      <c r="E24" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F24" s="62"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3104,7 +3204,9 @@
       <c r="D25" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="E25" s="65"/>
+      <c r="E25" s="65" t="s">
+        <v>20</v>
+      </c>
       <c r="F25" s="66"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3134,7 +3236,9 @@
         <v>174</v>
       </c>
       <c r="D27" s="54"/>
-      <c r="E27" s="63"/>
+      <c r="E27" s="63" t="s">
+        <v>20</v>
+      </c>
       <c r="F27" s="64"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,7 +3248,9 @@
       </c>
       <c r="C28" s="67"/>
       <c r="D28" s="59"/>
-      <c r="E28" s="61"/>
+      <c r="E28" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F28" s="62"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3154,7 +3260,9 @@
       </c>
       <c r="C29" s="67"/>
       <c r="D29" s="59"/>
-      <c r="E29" s="61"/>
+      <c r="E29" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F29" s="62"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3164,7 +3272,9 @@
         <v>73</v>
       </c>
       <c r="D30" s="59"/>
-      <c r="E30" s="61"/>
+      <c r="E30" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F30" s="62"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3174,7 +3284,9 @@
         <v>122</v>
       </c>
       <c r="D31" s="59"/>
-      <c r="E31" s="61"/>
+      <c r="E31" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F31" s="62"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3184,7 +3296,9 @@
         <v>112</v>
       </c>
       <c r="D32" s="59"/>
-      <c r="E32" s="61"/>
+      <c r="E32" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F32" s="62"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3196,7 +3310,9 @@
       <c r="D33" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="E33" s="65"/>
+      <c r="E33" s="65" t="s">
+        <v>20</v>
+      </c>
       <c r="F33" s="66"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,7 +3376,9 @@
         <v>109</v>
       </c>
       <c r="D38" s="59"/>
-      <c r="E38" s="61"/>
+      <c r="E38" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F38" s="62"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3418,7 +3536,9 @@
         <v>78</v>
       </c>
       <c r="D52" s="59"/>
-      <c r="E52" s="61"/>
+      <c r="E52" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F52" s="62"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Diseño de pruebas funcionalidades de puntaje en Juego
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D060690-6F7B-411A-83EC-A52731E69B50}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C428B630-DFE5-4CD6-A273-6AF79A865D17}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="192">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2784,7 +2784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -3462,7 +3462,9 @@
         <v>89</v>
       </c>
       <c r="D45" s="59"/>
-      <c r="E45" s="61"/>
+      <c r="E45" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F45" s="62"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3472,7 +3474,9 @@
         <v>79</v>
       </c>
       <c r="D46" s="59"/>
-      <c r="E46" s="61"/>
+      <c r="E46" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F46" s="62"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Diseño de pruebas funcionalidades de guardado y serialización elementos del juego
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C428B630-DFE5-4CD6-A273-6AF79A865D17}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0A6847-5B14-4770-940C-C200188C4844}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="192">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2784,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3392,7 +3392,9 @@
       <c r="D39" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F39" s="62"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3404,7 +3406,9 @@
       <c r="D40" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="61"/>
+      <c r="E40" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F40" s="62"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3416,7 +3420,9 @@
       <c r="D41" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="61"/>
+      <c r="E41" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F41" s="62"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3428,7 +3434,9 @@
       <c r="D42" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="61"/>
+      <c r="E42" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F42" s="62"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3440,7 +3448,9 @@
       <c r="D43" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="61"/>
+      <c r="E43" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F43" s="62"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Diseño de pruebas manejo archivos de texto
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0A6847-5B14-4770-940C-C200188C4844}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F588BB-D361-4FE0-875D-5A8CBB71E1C3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="192">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2056,7 +2056,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2793,8 @@
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="5"/>
+    <col min="5" max="5" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3462,7 +3463,9 @@
       <c r="D44" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="61"/>
+      <c r="E44" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F44" s="62"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Diseño de pruebas funcionalidades del cicloJuego
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F588BB-D361-4FE0-875D-5A8CBB71E1C3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91B5BD3-3DD7-4658-9020-ABDD9787107B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="192">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2784,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,7 +3513,9 @@
         <v>80</v>
       </c>
       <c r="D48" s="59"/>
-      <c r="E48" s="61"/>
+      <c r="E48" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F48" s="62"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3523,7 +3525,9 @@
         <v>90</v>
       </c>
       <c r="D49" s="59"/>
-      <c r="E49" s="61"/>
+      <c r="E49" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F49" s="62"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3533,7 +3537,9 @@
         <v>77</v>
       </c>
       <c r="D50" s="59"/>
-      <c r="E50" s="61"/>
+      <c r="E50" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F50" s="62"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3543,7 +3549,9 @@
         <v>81</v>
       </c>
       <c r="D51" s="59"/>
-      <c r="E51" s="61"/>
+      <c r="E51" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F51" s="62"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fin de diseño de pruebas
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91B5BD3-3DD7-4658-9020-ABDD9787107B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB71EA02-3CA4-428A-BE89-FC41D3C4591A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="195">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>dy</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>fuerte</t>
+  </si>
+  <si>
+    <t>rapido</t>
   </si>
 </sst>
 </file>
@@ -2782,10 +2791,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,7 +2807,7 @@
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>152</v>
       </c>
@@ -2824,7 +2833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>66</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="50" t="s">
         <v>140</v>
@@ -2863,8 +2872,11 @@
       <c r="I3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="50" t="s">
         <v>141</v>
@@ -2882,7 +2894,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="50" t="s">
         <v>142</v>
@@ -2894,7 +2906,7 @@
       </c>
       <c r="F5" s="62"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="50" t="s">
         <v>143</v>
@@ -2909,11 +2921,11 @@
         <v>186</v>
       </c>
       <c r="I6">
-        <f>I3-I1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <f>I3-I1+J3/2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="50"/>
       <c r="C7" s="48" t="s">
@@ -2930,11 +2942,11 @@
         <v>187</v>
       </c>
       <c r="I7">
-        <f>I4-I2</f>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <f>I4-I2+J3/2</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="74" t="s">
         <v>182</v>
@@ -2950,7 +2962,7 @@
       </c>
       <c r="F8" s="62"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="74"/>
       <c r="C9" s="48" t="s">
@@ -2968,10 +2980,10 @@
       </c>
       <c r="I9">
         <f>SQRT(I6*I6+I7*I7)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36.055512754639892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
       <c r="B10" s="50"/>
       <c r="C10" s="48" t="s">
@@ -2986,11 +2998,11 @@
         <v>189</v>
       </c>
       <c r="I10">
-        <f>20/I9</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>I16/I9</f>
+        <v>0.41602514716892186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="53"/>
       <c r="B11" s="51"/>
       <c r="C11" s="49" t="s">
@@ -3004,7 +3016,7 @@
       </c>
       <c r="F11" s="66"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>125</v>
       </c>
@@ -3027,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53"/>
       <c r="B13" s="51"/>
       <c r="C13" s="49" t="s">
@@ -3045,10 +3057,10 @@
       </c>
       <c r="I13">
         <f>I10*(I4-I2)</f>
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-20.801257358446094</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>70</v>
       </c>
@@ -3062,7 +3074,7 @@
       </c>
       <c r="F14" s="64"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
       <c r="B15" s="50"/>
       <c r="C15" s="48" t="s">
@@ -3076,7 +3088,7 @@
       </c>
       <c r="F15" s="62"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
       <c r="B16" s="50"/>
       <c r="C16" s="48" t="s">
@@ -3089,8 +3101,14 @@
         <v>20</v>
       </c>
       <c r="F16" s="62"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>193</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
       <c r="B17" s="50"/>
       <c r="C17" s="48" t="s">
@@ -3101,8 +3119,14 @@
         <v>20</v>
       </c>
       <c r="F17" s="62"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
       <c r="B18" s="50"/>
       <c r="C18" s="48" t="s">
@@ -3115,8 +3139,14 @@
         <v>20</v>
       </c>
       <c r="F18" s="62"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
       <c r="B19" s="50"/>
       <c r="C19" s="48" t="s">
@@ -3128,7 +3158,7 @@
       </c>
       <c r="F19" s="62"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="52"/>
       <c r="B20" s="50"/>
       <c r="C20" s="48" t="s">
@@ -3142,7 +3172,7 @@
       </c>
       <c r="F20" s="62"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
       <c r="B21" s="51"/>
       <c r="C21" s="49" t="s">
@@ -3154,7 +3184,7 @@
       </c>
       <c r="F21" s="66"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>69</v>
       </c>
@@ -3170,7 +3200,7 @@
       </c>
       <c r="F22" s="64"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="52"/>
       <c r="B23" s="50"/>
       <c r="C23" s="48" t="s">
@@ -3182,7 +3212,7 @@
       </c>
       <c r="F23" s="62"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="52"/>
       <c r="B24" s="50"/>
       <c r="C24" s="48" t="s">
@@ -3196,7 +3226,7 @@
       </c>
       <c r="F24" s="62"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
       <c r="B25" s="51"/>
       <c r="C25" s="49" t="s">
@@ -3210,7 +3240,7 @@
       </c>
       <c r="F25" s="66"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="60" t="s">
         <v>68</v>
       </c>
@@ -3226,7 +3256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
         <v>123</v>
       </c>
@@ -3242,7 +3272,7 @@
       </c>
       <c r="F27" s="64"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="52"/>
       <c r="B28" s="50" t="s">
         <v>146</v>
@@ -3254,7 +3284,7 @@
       </c>
       <c r="F28" s="62"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52"/>
       <c r="B29" s="50" t="s">
         <v>147</v>
@@ -3266,7 +3296,7 @@
       </c>
       <c r="F29" s="62"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="52"/>
       <c r="B30" s="50"/>
       <c r="C30" s="48" t="s">
@@ -3278,7 +3308,7 @@
       </c>
       <c r="F30" s="62"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="52"/>
       <c r="B31" s="50"/>
       <c r="C31" s="48" t="s">
@@ -3290,7 +3320,7 @@
       </c>
       <c r="F31" s="62"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52"/>
       <c r="B32" s="50"/>
       <c r="C32" s="48" t="s">

</xml_diff>

<commit_message>
Se empezó las pruebas del proyectil
Aun faltan pruebas de las bonificaciones
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ABB706-5FA9-46A3-A829-BABAA608A49D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF733318-81D1-470A-B6EB-0D2045199544}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2793,8 +2793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2947,9 +2947,7 @@
       <c r="E7" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="62" t="s">
-        <v>20</v>
-      </c>
+      <c r="F7" s="62"/>
       <c r="H7" t="s">
         <v>187</v>
       </c>
@@ -2972,9 +2970,7 @@
       <c r="E8" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="62" t="s">
-        <v>20</v>
-      </c>
+      <c r="F8" s="62"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -2988,9 +2984,7 @@
       <c r="E9" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="62" t="s">
-        <v>20</v>
-      </c>
+      <c r="F9" s="62"/>
       <c r="H9" t="s">
         <v>188</v>
       </c>
@@ -3294,7 +3288,9 @@
       <c r="E27" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="64"/>
+      <c r="F27" s="64" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="52"/>
@@ -3306,7 +3302,9 @@
       <c r="E28" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="62"/>
+      <c r="F28" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52"/>
@@ -3318,7 +3316,9 @@
       <c r="E29" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="62"/>
+      <c r="F29" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="52"/>

</xml_diff>

<commit_message>
Implementacion pruebas disparar Proyectil
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF733318-81D1-470A-B6EB-0D2045199544}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF25A2B-A3A7-4583-98AD-B89AB87F387E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="195">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2065,7 +2065,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,7 +2079,9 @@
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="38" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2103,7 +2105,9 @@
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" s="24" t="s">
         <v>135</v>
       </c>
@@ -2794,7 +2798,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2830,7 +2834,7 @@
         <v>20</v>
       </c>
       <c r="I1">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2854,7 +2858,7 @@
         <v>183</v>
       </c>
       <c r="I2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2897,7 +2901,7 @@
         <v>185</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2931,8 +2935,8 @@
         <v>186</v>
       </c>
       <c r="I6">
-        <f>I3-I1+J3/2</f>
-        <v>20</v>
+        <f>I3-I1+(J3/2)</f>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2947,13 +2951,15 @@
       <c r="E7" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="62"/>
+      <c r="F7" s="62" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" t="s">
         <v>187</v>
       </c>
       <c r="I7">
         <f>I4-I2+J3/2</f>
-        <v>-30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2970,7 +2976,9 @@
       <c r="E8" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="62"/>
+      <c r="F8" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -2984,13 +2992,15 @@
       <c r="E9" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="62"/>
+      <c r="F9" s="62" t="s">
+        <v>20</v>
+      </c>
       <c r="H9" t="s">
         <v>188</v>
       </c>
       <c r="I9">
         <f>SQRT(I6*I6+I7*I7)</f>
-        <v>36.055512754639892</v>
+        <v>98.994949366116657</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3010,8 +3020,8 @@
         <v>189</v>
       </c>
       <c r="I10">
-        <f>I16/I9</f>
-        <v>0.41602514716892186</v>
+        <f>I18/I9</f>
+        <v>0.2525381361380527</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3052,7 +3062,7 @@
       </c>
       <c r="I12">
         <f>I10*(I3-I1)</f>
-        <v>0</v>
+        <v>12.626906806902635</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3075,7 +3085,7 @@
       </c>
       <c r="I13">
         <f>I10*(I4-I2)</f>
-        <v>-20.801257358446094</v>
+        <v>12.626906806902635</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3330,7 +3340,9 @@
       <c r="E30" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="62"/>
+      <c r="F30" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="52"/>
@@ -3414,7 +3426,9 @@
       <c r="E36" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="62"/>
+      <c r="F36" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="52"/>
@@ -3426,7 +3440,9 @@
       <c r="E37" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="62"/>
+      <c r="F37" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="52"/>

</xml_diff>

<commit_message>
Creadas pruebas de Nave
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF733318-81D1-470A-B6EB-0D2045199544}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7558744E-FA9A-4F4F-BF7E-15A30AD72B6E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <sheet name="PruebasUnit" sheetId="6" r:id="rId5"/>
     <sheet name="JavaDoc" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="195">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2793,8 +2793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2947,7 +2947,9 @@
       <c r="E7" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="62"/>
+      <c r="F7" s="62" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" t="s">
         <v>187</v>
       </c>
@@ -2970,7 +2972,9 @@
       <c r="E8" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="62"/>
+      <c r="F8" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -2984,7 +2988,9 @@
       <c r="E9" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="62"/>
+      <c r="F9" s="62" t="s">
+        <v>20</v>
+      </c>
       <c r="H9" t="s">
         <v>188</v>
       </c>
@@ -3216,7 +3222,9 @@
       <c r="E22" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="64"/>
+      <c r="F22" s="64" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="52"/>
@@ -3228,7 +3236,9 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="62"/>
+      <c r="F23" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="52"/>
@@ -3242,7 +3252,9 @@
       <c r="E24" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="62"/>
+      <c r="F24" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>

</xml_diff>

<commit_message>
Pruebas manejo archivos de texto
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C39DED1-3BDB-4EEA-9660-8F01B48D6544}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497248D3-D6C0-46BB-B213-B7DE42E0F3CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="195">
   <si>
     <t>R1. Mover la nave en el campo</t>
   </si>
@@ -2797,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C61316-8C98-41D7-8D5B-3F7087B60642}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3484,7 +3484,9 @@
       <c r="E39" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="62"/>
+      <c r="F39" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="52"/>
@@ -3498,7 +3500,9 @@
       <c r="E40" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="62"/>
+      <c r="F40" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="52"/>
@@ -3512,7 +3516,9 @@
       <c r="E41" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="62"/>
+      <c r="F41" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="52"/>
@@ -3526,7 +3532,9 @@
       <c r="E42" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="62"/>
+      <c r="F42" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="52"/>
@@ -3540,7 +3548,9 @@
       <c r="E43" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="62"/>
+      <c r="F43" s="62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="52"/>

</xml_diff>